<commit_message>
updated io and industry files
</commit_message>
<xml_diff>
--- a/InputData/io-model/BVAbIC/BAU Value Added by ISIC Code.xlsx
+++ b/InputData/io-model/BVAbIC/BAU Value Added by ISIC Code.xlsx
@@ -391,6 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -417,7 +418,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1020,7 +1020,7 @@
           <t>BVAbIC BAU Value Added by ISIC Code</t>
         </is>
       </c>
-      <c r="C1" s="48" t="n">
+      <c r="C1" s="38" t="n">
         <v>44307</v>
       </c>
     </row>
@@ -1221,240 +1221,240 @@
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="38" t="inlineStr">
+      <c r="A3" s="39" t="inlineStr">
         <is>
           <t>Variable</t>
         </is>
       </c>
-      <c r="B3" s="39" t="n"/>
-      <c r="C3" s="43" t="inlineStr">
+      <c r="B3" s="40" t="n"/>
+      <c r="C3" s="44" t="inlineStr">
         <is>
           <t>TTL: Total</t>
         </is>
       </c>
-      <c r="D3" s="41" t="n"/>
-      <c r="E3" s="41" t="n"/>
-      <c r="F3" s="41" t="n"/>
-      <c r="G3" s="41" t="n"/>
-      <c r="H3" s="41" t="n"/>
-      <c r="I3" s="41" t="n"/>
-      <c r="J3" s="41" t="n"/>
-      <c r="K3" s="41" t="n"/>
-      <c r="L3" s="41" t="n"/>
-      <c r="M3" s="41" t="n"/>
-      <c r="N3" s="41" t="n"/>
-      <c r="O3" s="41" t="n"/>
-      <c r="P3" s="41" t="n"/>
-      <c r="Q3" s="41" t="n"/>
-      <c r="R3" s="41" t="n"/>
-      <c r="S3" s="41" t="n"/>
-      <c r="T3" s="41" t="n"/>
-      <c r="U3" s="41" t="n"/>
-      <c r="V3" s="41" t="n"/>
-      <c r="W3" s="41" t="n"/>
-      <c r="X3" s="41" t="n"/>
-      <c r="Y3" s="41" t="n"/>
-      <c r="Z3" s="41" t="n"/>
-      <c r="AA3" s="41" t="n"/>
-      <c r="AB3" s="41" t="n"/>
-      <c r="AC3" s="41" t="n"/>
-      <c r="AD3" s="41" t="n"/>
-      <c r="AE3" s="41" t="n"/>
-      <c r="AF3" s="41" t="n"/>
-      <c r="AG3" s="41" t="n"/>
-      <c r="AH3" s="41" t="n"/>
-      <c r="AI3" s="41" t="n"/>
-      <c r="AJ3" s="41" t="n"/>
-      <c r="AK3" s="41" t="n"/>
-      <c r="AL3" s="41" t="n"/>
-      <c r="AM3" s="41" t="n"/>
-      <c r="AN3" s="41" t="n"/>
-      <c r="AO3" s="41" t="n"/>
-      <c r="AP3" s="41" t="n"/>
-      <c r="AQ3" s="41" t="n"/>
-      <c r="AR3" s="41" t="n"/>
-      <c r="AS3" s="41" t="n"/>
-      <c r="AT3" s="41" t="n"/>
-      <c r="AU3" s="39" t="n"/>
+      <c r="D3" s="42" t="n"/>
+      <c r="E3" s="42" t="n"/>
+      <c r="F3" s="42" t="n"/>
+      <c r="G3" s="42" t="n"/>
+      <c r="H3" s="42" t="n"/>
+      <c r="I3" s="42" t="n"/>
+      <c r="J3" s="42" t="n"/>
+      <c r="K3" s="42" t="n"/>
+      <c r="L3" s="42" t="n"/>
+      <c r="M3" s="42" t="n"/>
+      <c r="N3" s="42" t="n"/>
+      <c r="O3" s="42" t="n"/>
+      <c r="P3" s="42" t="n"/>
+      <c r="Q3" s="42" t="n"/>
+      <c r="R3" s="42" t="n"/>
+      <c r="S3" s="42" t="n"/>
+      <c r="T3" s="42" t="n"/>
+      <c r="U3" s="42" t="n"/>
+      <c r="V3" s="42" t="n"/>
+      <c r="W3" s="42" t="n"/>
+      <c r="X3" s="42" t="n"/>
+      <c r="Y3" s="42" t="n"/>
+      <c r="Z3" s="42" t="n"/>
+      <c r="AA3" s="42" t="n"/>
+      <c r="AB3" s="42" t="n"/>
+      <c r="AC3" s="42" t="n"/>
+      <c r="AD3" s="42" t="n"/>
+      <c r="AE3" s="42" t="n"/>
+      <c r="AF3" s="42" t="n"/>
+      <c r="AG3" s="42" t="n"/>
+      <c r="AH3" s="42" t="n"/>
+      <c r="AI3" s="42" t="n"/>
+      <c r="AJ3" s="42" t="n"/>
+      <c r="AK3" s="42" t="n"/>
+      <c r="AL3" s="42" t="n"/>
+      <c r="AM3" s="42" t="n"/>
+      <c r="AN3" s="42" t="n"/>
+      <c r="AO3" s="42" t="n"/>
+      <c r="AP3" s="42" t="n"/>
+      <c r="AQ3" s="42" t="n"/>
+      <c r="AR3" s="42" t="n"/>
+      <c r="AS3" s="42" t="n"/>
+      <c r="AT3" s="42" t="n"/>
+      <c r="AU3" s="40" t="n"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="38" t="inlineStr">
+      <c r="A4" s="39" t="inlineStr">
         <is>
           <t>Country</t>
         </is>
       </c>
-      <c r="B4" s="39" t="n"/>
-      <c r="C4" s="40" t="inlineStr">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="41" t="inlineStr">
         <is>
           <t>USA: United States</t>
         </is>
       </c>
-      <c r="D4" s="41" t="n"/>
-      <c r="E4" s="41" t="n"/>
-      <c r="F4" s="41" t="n"/>
-      <c r="G4" s="41" t="n"/>
-      <c r="H4" s="41" t="n"/>
-      <c r="I4" s="41" t="n"/>
-      <c r="J4" s="41" t="n"/>
-      <c r="K4" s="41" t="n"/>
-      <c r="L4" s="41" t="n"/>
-      <c r="M4" s="41" t="n"/>
-      <c r="N4" s="41" t="n"/>
-      <c r="O4" s="41" t="n"/>
-      <c r="P4" s="41" t="n"/>
-      <c r="Q4" s="41" t="n"/>
-      <c r="R4" s="41" t="n"/>
-      <c r="S4" s="41" t="n"/>
-      <c r="T4" s="41" t="n"/>
-      <c r="U4" s="41" t="n"/>
-      <c r="V4" s="41" t="n"/>
-      <c r="W4" s="41" t="n"/>
-      <c r="X4" s="41" t="n"/>
-      <c r="Y4" s="41" t="n"/>
-      <c r="Z4" s="41" t="n"/>
-      <c r="AA4" s="41" t="n"/>
-      <c r="AB4" s="41" t="n"/>
-      <c r="AC4" s="41" t="n"/>
-      <c r="AD4" s="41" t="n"/>
-      <c r="AE4" s="41" t="n"/>
-      <c r="AF4" s="41" t="n"/>
-      <c r="AG4" s="41" t="n"/>
-      <c r="AH4" s="41" t="n"/>
-      <c r="AI4" s="41" t="n"/>
-      <c r="AJ4" s="41" t="n"/>
-      <c r="AK4" s="41" t="n"/>
-      <c r="AL4" s="41" t="n"/>
-      <c r="AM4" s="41" t="n"/>
-      <c r="AN4" s="41" t="n"/>
-      <c r="AO4" s="41" t="n"/>
-      <c r="AP4" s="41" t="n"/>
-      <c r="AQ4" s="41" t="n"/>
-      <c r="AR4" s="41" t="n"/>
-      <c r="AS4" s="41" t="n"/>
-      <c r="AT4" s="41" t="n"/>
-      <c r="AU4" s="39" t="n"/>
+      <c r="D4" s="42" t="n"/>
+      <c r="E4" s="42" t="n"/>
+      <c r="F4" s="42" t="n"/>
+      <c r="G4" s="42" t="n"/>
+      <c r="H4" s="42" t="n"/>
+      <c r="I4" s="42" t="n"/>
+      <c r="J4" s="42" t="n"/>
+      <c r="K4" s="42" t="n"/>
+      <c r="L4" s="42" t="n"/>
+      <c r="M4" s="42" t="n"/>
+      <c r="N4" s="42" t="n"/>
+      <c r="O4" s="42" t="n"/>
+      <c r="P4" s="42" t="n"/>
+      <c r="Q4" s="42" t="n"/>
+      <c r="R4" s="42" t="n"/>
+      <c r="S4" s="42" t="n"/>
+      <c r="T4" s="42" t="n"/>
+      <c r="U4" s="42" t="n"/>
+      <c r="V4" s="42" t="n"/>
+      <c r="W4" s="42" t="n"/>
+      <c r="X4" s="42" t="n"/>
+      <c r="Y4" s="42" t="n"/>
+      <c r="Z4" s="42" t="n"/>
+      <c r="AA4" s="42" t="n"/>
+      <c r="AB4" s="42" t="n"/>
+      <c r="AC4" s="42" t="n"/>
+      <c r="AD4" s="42" t="n"/>
+      <c r="AE4" s="42" t="n"/>
+      <c r="AF4" s="42" t="n"/>
+      <c r="AG4" s="42" t="n"/>
+      <c r="AH4" s="42" t="n"/>
+      <c r="AI4" s="42" t="n"/>
+      <c r="AJ4" s="42" t="n"/>
+      <c r="AK4" s="42" t="n"/>
+      <c r="AL4" s="42" t="n"/>
+      <c r="AM4" s="42" t="n"/>
+      <c r="AN4" s="42" t="n"/>
+      <c r="AO4" s="42" t="n"/>
+      <c r="AP4" s="42" t="n"/>
+      <c r="AQ4" s="42" t="n"/>
+      <c r="AR4" s="42" t="n"/>
+      <c r="AS4" s="42" t="n"/>
+      <c r="AT4" s="42" t="n"/>
+      <c r="AU4" s="40" t="n"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="38" t="inlineStr">
+      <c r="A5" s="39" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B5" s="39" t="n"/>
-      <c r="C5" s="40" t="inlineStr">
+      <c r="B5" s="40" t="n"/>
+      <c r="C5" s="41" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
       </c>
-      <c r="D5" s="41" t="n"/>
-      <c r="E5" s="41" t="n"/>
-      <c r="F5" s="41" t="n"/>
-      <c r="G5" s="41" t="n"/>
-      <c r="H5" s="41" t="n"/>
-      <c r="I5" s="41" t="n"/>
-      <c r="J5" s="41" t="n"/>
-      <c r="K5" s="41" t="n"/>
-      <c r="L5" s="41" t="n"/>
-      <c r="M5" s="41" t="n"/>
-      <c r="N5" s="41" t="n"/>
-      <c r="O5" s="41" t="n"/>
-      <c r="P5" s="41" t="n"/>
-      <c r="Q5" s="41" t="n"/>
-      <c r="R5" s="41" t="n"/>
-      <c r="S5" s="41" t="n"/>
-      <c r="T5" s="41" t="n"/>
-      <c r="U5" s="41" t="n"/>
-      <c r="V5" s="41" t="n"/>
-      <c r="W5" s="41" t="n"/>
-      <c r="X5" s="41" t="n"/>
-      <c r="Y5" s="41" t="n"/>
-      <c r="Z5" s="41" t="n"/>
-      <c r="AA5" s="41" t="n"/>
-      <c r="AB5" s="41" t="n"/>
-      <c r="AC5" s="41" t="n"/>
-      <c r="AD5" s="41" t="n"/>
-      <c r="AE5" s="41" t="n"/>
-      <c r="AF5" s="41" t="n"/>
-      <c r="AG5" s="41" t="n"/>
-      <c r="AH5" s="41" t="n"/>
-      <c r="AI5" s="41" t="n"/>
-      <c r="AJ5" s="41" t="n"/>
-      <c r="AK5" s="41" t="n"/>
-      <c r="AL5" s="41" t="n"/>
-      <c r="AM5" s="41" t="n"/>
-      <c r="AN5" s="41" t="n"/>
-      <c r="AO5" s="41" t="n"/>
-      <c r="AP5" s="41" t="n"/>
-      <c r="AQ5" s="41" t="n"/>
-      <c r="AR5" s="41" t="n"/>
-      <c r="AS5" s="41" t="n"/>
-      <c r="AT5" s="41" t="n"/>
-      <c r="AU5" s="39" t="n"/>
+      <c r="D5" s="42" t="n"/>
+      <c r="E5" s="42" t="n"/>
+      <c r="F5" s="42" t="n"/>
+      <c r="G5" s="42" t="n"/>
+      <c r="H5" s="42" t="n"/>
+      <c r="I5" s="42" t="n"/>
+      <c r="J5" s="42" t="n"/>
+      <c r="K5" s="42" t="n"/>
+      <c r="L5" s="42" t="n"/>
+      <c r="M5" s="42" t="n"/>
+      <c r="N5" s="42" t="n"/>
+      <c r="O5" s="42" t="n"/>
+      <c r="P5" s="42" t="n"/>
+      <c r="Q5" s="42" t="n"/>
+      <c r="R5" s="42" t="n"/>
+      <c r="S5" s="42" t="n"/>
+      <c r="T5" s="42" t="n"/>
+      <c r="U5" s="42" t="n"/>
+      <c r="V5" s="42" t="n"/>
+      <c r="W5" s="42" t="n"/>
+      <c r="X5" s="42" t="n"/>
+      <c r="Y5" s="42" t="n"/>
+      <c r="Z5" s="42" t="n"/>
+      <c r="AA5" s="42" t="n"/>
+      <c r="AB5" s="42" t="n"/>
+      <c r="AC5" s="42" t="n"/>
+      <c r="AD5" s="42" t="n"/>
+      <c r="AE5" s="42" t="n"/>
+      <c r="AF5" s="42" t="n"/>
+      <c r="AG5" s="42" t="n"/>
+      <c r="AH5" s="42" t="n"/>
+      <c r="AI5" s="42" t="n"/>
+      <c r="AJ5" s="42" t="n"/>
+      <c r="AK5" s="42" t="n"/>
+      <c r="AL5" s="42" t="n"/>
+      <c r="AM5" s="42" t="n"/>
+      <c r="AN5" s="42" t="n"/>
+      <c r="AO5" s="42" t="n"/>
+      <c r="AP5" s="42" t="n"/>
+      <c r="AQ5" s="42" t="n"/>
+      <c r="AR5" s="42" t="n"/>
+      <c r="AS5" s="42" t="n"/>
+      <c r="AT5" s="42" t="n"/>
+      <c r="AU5" s="40" t="n"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="38" t="inlineStr">
+      <c r="A6" s="39" t="inlineStr">
         <is>
           <t>Unit</t>
         </is>
       </c>
-      <c r="B6" s="39" t="n"/>
-      <c r="C6" s="40" t="inlineStr">
+      <c r="B6" s="40" t="n"/>
+      <c r="C6" s="41" t="inlineStr">
         <is>
           <t>US Dollar, Millions</t>
         </is>
       </c>
-      <c r="D6" s="41" t="n"/>
-      <c r="E6" s="41" t="n"/>
-      <c r="F6" s="41" t="n"/>
-      <c r="G6" s="41" t="n"/>
-      <c r="H6" s="41" t="n"/>
-      <c r="I6" s="41" t="n"/>
-      <c r="J6" s="41" t="n"/>
-      <c r="K6" s="41" t="n"/>
-      <c r="L6" s="41" t="n"/>
-      <c r="M6" s="41" t="n"/>
-      <c r="N6" s="41" t="n"/>
-      <c r="O6" s="41" t="n"/>
-      <c r="P6" s="41" t="n"/>
-      <c r="Q6" s="41" t="n"/>
-      <c r="R6" s="41" t="n"/>
-      <c r="S6" s="41" t="n"/>
-      <c r="T6" s="41" t="n"/>
-      <c r="U6" s="41" t="n"/>
-      <c r="V6" s="41" t="n"/>
-      <c r="W6" s="41" t="n"/>
-      <c r="X6" s="41" t="n"/>
-      <c r="Y6" s="41" t="n"/>
-      <c r="Z6" s="41" t="n"/>
-      <c r="AA6" s="41" t="n"/>
-      <c r="AB6" s="41" t="n"/>
-      <c r="AC6" s="41" t="n"/>
-      <c r="AD6" s="41" t="n"/>
-      <c r="AE6" s="41" t="n"/>
-      <c r="AF6" s="41" t="n"/>
-      <c r="AG6" s="41" t="n"/>
-      <c r="AH6" s="41" t="n"/>
-      <c r="AI6" s="41" t="n"/>
-      <c r="AJ6" s="41" t="n"/>
-      <c r="AK6" s="41" t="n"/>
-      <c r="AL6" s="41" t="n"/>
-      <c r="AM6" s="41" t="n"/>
-      <c r="AN6" s="41" t="n"/>
-      <c r="AO6" s="41" t="n"/>
-      <c r="AP6" s="41" t="n"/>
-      <c r="AQ6" s="41" t="n"/>
-      <c r="AR6" s="41" t="n"/>
-      <c r="AS6" s="41" t="n"/>
-      <c r="AT6" s="41" t="n"/>
-      <c r="AU6" s="39" t="n"/>
+      <c r="D6" s="42" t="n"/>
+      <c r="E6" s="42" t="n"/>
+      <c r="F6" s="42" t="n"/>
+      <c r="G6" s="42" t="n"/>
+      <c r="H6" s="42" t="n"/>
+      <c r="I6" s="42" t="n"/>
+      <c r="J6" s="42" t="n"/>
+      <c r="K6" s="42" t="n"/>
+      <c r="L6" s="42" t="n"/>
+      <c r="M6" s="42" t="n"/>
+      <c r="N6" s="42" t="n"/>
+      <c r="O6" s="42" t="n"/>
+      <c r="P6" s="42" t="n"/>
+      <c r="Q6" s="42" t="n"/>
+      <c r="R6" s="42" t="n"/>
+      <c r="S6" s="42" t="n"/>
+      <c r="T6" s="42" t="n"/>
+      <c r="U6" s="42" t="n"/>
+      <c r="V6" s="42" t="n"/>
+      <c r="W6" s="42" t="n"/>
+      <c r="X6" s="42" t="n"/>
+      <c r="Y6" s="42" t="n"/>
+      <c r="Z6" s="42" t="n"/>
+      <c r="AA6" s="42" t="n"/>
+      <c r="AB6" s="42" t="n"/>
+      <c r="AC6" s="42" t="n"/>
+      <c r="AD6" s="42" t="n"/>
+      <c r="AE6" s="42" t="n"/>
+      <c r="AF6" s="42" t="n"/>
+      <c r="AG6" s="42" t="n"/>
+      <c r="AH6" s="42" t="n"/>
+      <c r="AI6" s="42" t="n"/>
+      <c r="AJ6" s="42" t="n"/>
+      <c r="AK6" s="42" t="n"/>
+      <c r="AL6" s="42" t="n"/>
+      <c r="AM6" s="42" t="n"/>
+      <c r="AN6" s="42" t="n"/>
+      <c r="AO6" s="42" t="n"/>
+      <c r="AP6" s="42" t="n"/>
+      <c r="AQ6" s="42" t="n"/>
+      <c r="AR6" s="42" t="n"/>
+      <c r="AS6" s="42" t="n"/>
+      <c r="AT6" s="42" t="n"/>
+      <c r="AU6" s="40" t="n"/>
     </row>
     <row r="7" ht="126" customHeight="1">
-      <c r="A7" s="42" t="inlineStr">
+      <c r="A7" s="43" t="inlineStr">
         <is>
           <t>To: (sector in column)</t>
         </is>
       </c>
-      <c r="B7" s="39" t="n"/>
+      <c r="B7" s="40" t="n"/>
       <c r="C7" s="8" t="inlineStr">
         <is>
           <t>D01T03: Agriculture, forestry and fishing</t>
@@ -7664,80 +7664,80 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="45" t="inlineStr">
+      <c r="A3" s="46" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B3" s="39" t="n"/>
-      <c r="C3" s="46" t="inlineStr">
+      <c r="B3" s="40" t="n"/>
+      <c r="C3" s="47" t="inlineStr">
         <is>
           <t>2015</t>
         </is>
       </c>
-      <c r="D3" s="41" t="n"/>
-      <c r="E3" s="41" t="n"/>
-      <c r="F3" s="41" t="n"/>
-      <c r="G3" s="41" t="n"/>
-      <c r="H3" s="41" t="n"/>
-      <c r="I3" s="41" t="n"/>
-      <c r="J3" s="41" t="n"/>
-      <c r="K3" s="41" t="n"/>
-      <c r="L3" s="41" t="n"/>
-      <c r="M3" s="41" t="n"/>
-      <c r="N3" s="39" t="n"/>
+      <c r="D3" s="42" t="n"/>
+      <c r="E3" s="42" t="n"/>
+      <c r="F3" s="42" t="n"/>
+      <c r="G3" s="42" t="n"/>
+      <c r="H3" s="42" t="n"/>
+      <c r="I3" s="42" t="n"/>
+      <c r="J3" s="42" t="n"/>
+      <c r="K3" s="42" t="n"/>
+      <c r="L3" s="42" t="n"/>
+      <c r="M3" s="42" t="n"/>
+      <c r="N3" s="40" t="n"/>
     </row>
     <row r="4" ht="24" customHeight="1">
-      <c r="A4" s="44" t="inlineStr">
+      <c r="A4" s="45" t="inlineStr">
         <is>
           <t>Variable</t>
         </is>
       </c>
-      <c r="B4" s="39" t="n"/>
-      <c r="C4" s="47" t="inlineStr">
+      <c r="B4" s="40" t="n"/>
+      <c r="C4" s="48" t="inlineStr">
         <is>
           <t>PROD: Production (gross output), current prices</t>
         </is>
       </c>
-      <c r="D4" s="39" t="n"/>
-      <c r="E4" s="47" t="inlineStr">
+      <c r="D4" s="40" t="n"/>
+      <c r="E4" s="48" t="inlineStr">
         <is>
           <t>VALU: Value added, current prices</t>
         </is>
       </c>
-      <c r="F4" s="39" t="n"/>
-      <c r="G4" s="47" t="inlineStr">
+      <c r="F4" s="40" t="n"/>
+      <c r="G4" s="48" t="inlineStr">
         <is>
           <t>LABR: Labour costs (compensation of employees)</t>
         </is>
       </c>
-      <c r="H4" s="39" t="n"/>
-      <c r="I4" s="47" t="inlineStr">
+      <c r="H4" s="40" t="n"/>
+      <c r="I4" s="48" t="inlineStr">
         <is>
           <t>GOPS: Gross operating surplus and mixed income</t>
         </is>
       </c>
-      <c r="J4" s="39" t="n"/>
-      <c r="K4" s="47" t="inlineStr">
+      <c r="J4" s="40" t="n"/>
+      <c r="K4" s="48" t="inlineStr">
         <is>
           <t>OTXS: Other taxes less subsidies on production</t>
         </is>
       </c>
-      <c r="L4" s="39" t="n"/>
-      <c r="M4" s="47" t="inlineStr">
+      <c r="L4" s="40" t="n"/>
+      <c r="M4" s="48" t="inlineStr">
         <is>
           <t>EMPN: Number of persons engaged (total employment)</t>
         </is>
       </c>
-      <c r="N4" s="39" t="n"/>
+      <c r="N4" s="40" t="n"/>
     </row>
     <row r="5" ht="63" customHeight="1">
-      <c r="A5" s="44" t="inlineStr">
+      <c r="A5" s="45" t="inlineStr">
         <is>
           <t>Industry</t>
         </is>
       </c>
-      <c r="B5" s="39" t="n"/>
+      <c r="B5" s="40" t="n"/>
       <c r="C5" s="20" t="inlineStr">
         <is>
           <t>D20: Chemicals and chemical products [CE]</t>
@@ -9279,10 +9279,10 @@
         <v>745179114.3151599</v>
       </c>
       <c r="C2" s="33" t="n">
-        <v>4173657990.351198</v>
+        <v>257967316.3227949</v>
       </c>
       <c r="D2" s="34" t="n">
-        <v>69125607.96742155</v>
+        <v>1118384492.049778</v>
       </c>
       <c r="E2" t="n">
         <v>204807713.5615</v>

</xml_diff>